<commit_message>
the check is working. some minor fixes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t xml:space="preserve">jj7654321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jj100 device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJ150</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -185,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,26 +270,6 @@
         <v>41092</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>34234</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>41092</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -315,7 +289,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5:F5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,17 +299,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
normalize function returns a fixed width data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t xml:space="preserve">jj7654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jj100 device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JJ150</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -179,7 +185,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="A5:F5"/>
@@ -267,6 +273,26 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="n">
+        <v>41092</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>34234</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>41092</v>
       </c>
     </row>
@@ -299,17 +325,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
database sanity check in GUI and core
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -41,37 +41,55 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">new fun 100 device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JM100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JM199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New 20 devices’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JM200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jm299</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7digis “hi”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJ1000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jj7654321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jj100 device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJ150</t>
+    <t xml:space="preserve">row1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA0000000000000000000000000100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA0000000000000000000000000200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB0000000000000000000000000500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB0000000000000000000000000600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA0000000000000000000000000110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA0000000000000000000000000120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA0000000000000000000000000090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC0000000000000000000000000090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC0000000000000000000000000200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB0000000000000000000000000090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB0000000000000000000000001100</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -186,17 +204,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -224,7 +244,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>100</v>
+        <v>24234</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -232,7 +252,7 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="2" t="n">
@@ -243,10 +263,10 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="0" t="n">
+        <v>54365</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -256,17 +276,17 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>41092</v>
+        <v>41093</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="0" t="n">
+        <v>7567</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -276,27 +296,67 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>41092</v>
+        <v>41094</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>34234</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="0" t="n">
+        <v>578</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F5" s="2" t="n">
-        <v>41092</v>
+        <v>41095</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>41096</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>87654</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>41097</v>
       </c>
     </row>
   </sheetData>
@@ -328,17 +388,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user can see all sanity with url
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -89,7 +89,16 @@
     <t xml:space="preserve">AB0000000000000000000000000090</t>
   </si>
   <si>
-    <t xml:space="preserve">AB0000000000000000000000001100</t>
+    <t xml:space="preserve">AC0000000000000000000000001100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA00000000000000000000000000101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA0000000000000000000000000105</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -204,10 +213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,6 +366,26 @@
       </c>
       <c r="F7" s="2" t="n">
         <v>41097</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>45646</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>41095</v>
       </c>
     </row>
   </sheetData>
@@ -388,17 +417,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>